<commit_message>
added optional number column
</commit_message>
<xml_diff>
--- a/example/example_data.xlsx
+++ b/example/example_data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\hide\work\reg-vis\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4881F31-C82B-475E-8600-A5458BF42C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F3CB42-9361-476F-AAC4-0B17DD632180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Variable group</t>
   </si>
@@ -71,6 +84,9 @@
   </si>
   <si>
     <t>Brown</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -102,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -125,13 +141,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -472,18 +502,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,8 +533,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -516,8 +553,11 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -533,8 +573,11 @@
       <c r="E3">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -550,8 +593,11 @@
       <c r="E4">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -567,8 +613,11 @@
       <c r="E5">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -584,8 +633,11 @@
       <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -601,8 +653,11 @@
       <c r="E7">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -618,8 +673,11 @@
       <c r="E8">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -634,6 +692,9 @@
       </c>
       <c r="E9">
         <v>2.75</v>
+      </c>
+      <c r="F9">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to change result name
</commit_message>
<xml_diff>
--- a/example/example_data.xlsx
+++ b/example/example_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\hide\work\reg-vis\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE25FE0-85A7-4871-8D6D-D09B2ABE50EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E7AA97-E554-4C8E-8474-1BDA8A25774B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="864" yWindow="2856" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Variable</t>
   </si>
   <si>
-    <t>Odds Ratio</t>
-  </si>
-  <si>
     <t>Conf int upper</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -149,7 +149,9 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -505,7 +507,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,33 +527,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>103</v>
@@ -559,10 +561,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>2.2999999999999998</v>
@@ -579,10 +581,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1.3</v>
@@ -599,10 +601,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>2.7</v>
@@ -619,10 +621,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -639,10 +641,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
       <c r="C7">
         <v>2.4</v>
@@ -659,10 +661,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>2.2999999999999998</v>
@@ -679,10 +681,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>2.4</v>

</xml_diff>